<commit_message>
Entity Column Names to upperCase
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelberger/Developer/projects/ExcelPOIHelper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99415E2-8C9E-9B4D-9680-F5590A771EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8711C0C0-F634-9C46-B716-BDA428851493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="1800" windowWidth="28240" windowHeight="17560" activeTab="1" xr2:uid="{C51E43B3-2B3C-0447-B8A2-09DBEF823A5D}"/>
   </bookViews>
@@ -34,12 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>sdfsdf</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>ERER_ERER_FDF</t>
+    <t>MODEL_Name</t>
+  </si>
+  <si>
+    <t>MODEL_ART</t>
+  </si>
+  <si>
+    <t>Model_tYp</t>
+  </si>
+  <si>
+    <t>modEL_NuMBER</t>
   </si>
 </sst>
 </file>
@@ -403,35 +412,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4408FD50-037E-B647-B2B0-D24C18AC5518}">
-  <dimension ref="A2:L2"/>
+  <dimension ref="A2:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>